<commit_message>
Modification de la page liste de profils et ajout d'une description à toutes les ressources 8529e341a78e81150f1aac9ee97d54ec6d7e597c
</commit_message>
<xml_diff>
--- a/180-rc-synthèse-des-ressources/ig/StructureDefinition-esms-bundle-resultat-recherche-decision-evaluation.xlsx
+++ b/180-rc-synthèse-des-ressources/ig/StructureDefinition-esms-bundle-resultat-recherche-decision-evaluation.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-09-30T09:02:08+00:00</t>
+    <t>2024-09-30T11:49:20+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -78,7 +78,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Profil pour la définition du Bundle de réponse à la recherche d'une décision d'orientation ou d'une évaluation</t>
+    <t>Profil ESMS pour la définition du Bundle de réponse à la recherche d'une décision d'orientation ou d'une évaluation</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>

<commit_message>
Correction description SD 701680b9074bd0112982efadd03b45c0aaf2cd8d
</commit_message>
<xml_diff>
--- a/180-rc-synthèse-des-ressources/ig/StructureDefinition-esms-bundle-resultat-recherche-decision-evaluation.xlsx
+++ b/180-rc-synthèse-des-ressources/ig/StructureDefinition-esms-bundle-resultat-recherche-decision-evaluation.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-10-01T07:24:36+00:00</t>
+    <t>2024-10-01T08:28:09+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -78,7 +78,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Profil ESMS pour la définition du Bundle de réponse à la recherche d'une décision d'orientation ou d'une évaluation</t>
+    <t>Profil ESMS créé dans le contexte du suivi des orientations pour transporter les documents répondant à une recherche de decision ou d’évaluation. Il repose sur le profil ESMSDocumentReference.</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>